<commit_message>
Working on cart functionality
</commit_message>
<xml_diff>
--- a/src/main/resources/sampleExcelFormat.xlsx
+++ b/src/main/resources/sampleExcelFormat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svasu\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Express-Grocery\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EFC5F7-DDFB-46D7-8376-85576BF094EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C731CC6-5237-4B43-BA8F-4C203365EA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22930" yWindow="-110" windowWidth="23260" windowHeight="12460" xr2:uid="{C25201F3-BE9A-4908-BAB6-F136034A5821}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C25201F3-BE9A-4908-BAB6-F136034A5821}"/>
   </bookViews>
   <sheets>
     <sheet name="product_data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>S no</t>
   </si>
@@ -77,10 +77,16 @@
     <t>category</t>
   </si>
   <si>
-    <t>School Items, stationary</t>
-  </si>
-  <si>
     <t>bag</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Toys</t>
+  </si>
+  <si>
+    <t>Electronics, Toys</t>
   </si>
 </sst>
 </file>
@@ -124,7 +130,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -464,7 +470,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -474,7 +480,7 @@
     <col min="3" max="3" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.90625" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.54296875" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.7265625" style="1"/>
@@ -496,7 +502,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -506,12 +512,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -522,11 +528,11 @@
       <c r="E2" s="2">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="b">
+      <c r="F2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
+      <c r="H2" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -545,8 +551,11 @@
       <c r="E3" s="2">
         <v>10</v>
       </c>
-      <c r="F3" s="3" t="b">
+      <c r="F3" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -565,8 +574,11 @@
       <c r="E4" s="2">
         <v>2</v>
       </c>
-      <c r="F4" s="3" t="b">
+      <c r="F4" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>